<commit_message>
mudanças na estrutura das datas
</commit_message>
<xml_diff>
--- a/data/raw-data.xlsx
+++ b/data/raw-data.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'raw-data'!$A$1:$J$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'raw-data'!$A$1:$L$31</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -105,9 +105,6 @@
     <t>name.genus</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>collected</t>
   </si>
   <si>
@@ -184,6 +181,15 @@
   </si>
   <si>
     <t>verticillata</t>
+  </si>
+  <si>
+    <t>date.year</t>
+  </si>
+  <si>
+    <t>date.month</t>
+  </si>
+  <si>
+    <t>date.day</t>
   </si>
 </sst>
 </file>
@@ -221,7 +227,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,27 +529,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,20 +568,26 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -595,19 +607,25 @@
         <v>12</v>
       </c>
       <c r="G2" s="1">
-        <v>42593</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>40</v>
+        <v>2016</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1">
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -627,16 +645,22 @@
         <v>14</v>
       </c>
       <c r="G3" s="1">
-        <v>42593</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H3" s="1">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -656,13 +680,19 @@
         <v>14</v>
       </c>
       <c r="G4" s="1">
-        <v>42593</v>
-      </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -682,13 +712,19 @@
         <v>14</v>
       </c>
       <c r="G5" s="1">
-        <v>42593</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H5" s="1">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -708,16 +744,22 @@
         <v>17</v>
       </c>
       <c r="G6" s="1">
-        <v>42593</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H6" s="1">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -737,16 +779,22 @@
         <v>17</v>
       </c>
       <c r="G7" s="1">
-        <v>42595</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
+        <v>2016</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1">
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -763,19 +811,25 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1">
-        <v>42595</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -795,13 +849,19 @@
         <v>17</v>
       </c>
       <c r="G9" s="1">
-        <v>42595</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H9" s="1">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -818,16 +878,22 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1">
-        <v>42595</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H10" s="1">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -847,13 +913,19 @@
         <v>17</v>
       </c>
       <c r="G11" s="1">
-        <v>42595</v>
-      </c>
-      <c r="H11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H11" s="1">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -870,19 +942,25 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1">
-        <v>42597</v>
-      </c>
-      <c r="H12" t="s">
-        <v>32</v>
+        <v>2016</v>
+      </c>
+      <c r="H12" s="1">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1">
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -902,13 +980,19 @@
         <v>17</v>
       </c>
       <c r="G13" s="1">
-        <v>42597</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H13" s="1">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -928,13 +1012,19 @@
         <v>17</v>
       </c>
       <c r="G14" s="1">
-        <v>42597</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H14" s="1">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -954,13 +1044,19 @@
         <v>17</v>
       </c>
       <c r="G15" s="1">
-        <v>42597</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H15" s="1">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -980,13 +1076,19 @@
         <v>17</v>
       </c>
       <c r="G16" s="1">
-        <v>42597</v>
-      </c>
-      <c r="H16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1006,19 +1108,25 @@
         <v>19</v>
       </c>
       <c r="G17" s="1">
-        <v>42599</v>
-      </c>
-      <c r="H17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" t="s">
-        <v>44</v>
+        <v>2016</v>
+      </c>
+      <c r="H17" s="1">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1">
+        <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1038,13 +1146,19 @@
         <v>12</v>
       </c>
       <c r="G18" s="1">
-        <v>42599</v>
-      </c>
-      <c r="H18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H18" s="1">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1064,13 +1178,19 @@
         <v>19</v>
       </c>
       <c r="G19" s="1">
-        <v>42599</v>
-      </c>
-      <c r="H19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H19" s="1">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1090,13 +1210,19 @@
         <v>12</v>
       </c>
       <c r="G20" s="1">
-        <v>42599</v>
-      </c>
-      <c r="H20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H20" s="1">
+        <v>8</v>
+      </c>
+      <c r="I20" s="1">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1116,13 +1242,19 @@
         <v>12</v>
       </c>
       <c r="G21" s="1">
-        <v>42599</v>
-      </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H21" s="1">
+        <v>8</v>
+      </c>
+      <c r="I21" s="1">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1142,16 +1274,22 @@
         <v>19</v>
       </c>
       <c r="G22" s="1">
-        <v>42601</v>
-      </c>
-      <c r="H22" t="s">
-        <v>32</v>
+        <v>2016</v>
+      </c>
+      <c r="H22" s="1">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1">
+        <v>15</v>
       </c>
       <c r="J22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="L22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1171,13 +1309,19 @@
         <v>19</v>
       </c>
       <c r="G23" s="1">
-        <v>42601</v>
-      </c>
-      <c r="H23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H23" s="1">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1">
+        <v>15</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1197,16 +1341,22 @@
         <v>21</v>
       </c>
       <c r="G24" s="1">
-        <v>42601</v>
-      </c>
-      <c r="H24" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H24" s="1">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1">
+        <v>15</v>
+      </c>
+      <c r="J24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1226,16 +1376,22 @@
         <v>21</v>
       </c>
       <c r="G25" s="1">
-        <v>42601</v>
-      </c>
-      <c r="H25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H25" s="1">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1">
+        <v>15</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1255,13 +1411,19 @@
         <v>14</v>
       </c>
       <c r="G26" s="1">
-        <v>42601</v>
-      </c>
-      <c r="H26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H26" s="1">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1">
+        <v>15</v>
+      </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1269,31 +1431,37 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
       </c>
       <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
         <v>49</v>
       </c>
-      <c r="F27" t="s">
-        <v>50</v>
-      </c>
       <c r="G27" s="1">
-        <v>42603</v>
-      </c>
-      <c r="H27" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" t="s">
-        <v>45</v>
+        <v>2016</v>
+      </c>
+      <c r="H27" s="1">
+        <v>8</v>
+      </c>
+      <c r="I27" s="1">
+        <v>17</v>
       </c>
       <c r="J27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K27" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1301,25 +1469,31 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
       </c>
       <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s">
         <v>49</v>
       </c>
-      <c r="F28" t="s">
-        <v>50</v>
-      </c>
       <c r="G28" s="1">
-        <v>42603</v>
-      </c>
-      <c r="H28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H28" s="1">
+        <v>8</v>
+      </c>
+      <c r="I28" s="1">
+        <v>17</v>
+      </c>
+      <c r="J28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1327,28 +1501,34 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
       </c>
       <c r="E29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" t="s">
         <v>51</v>
       </c>
-      <c r="F29" t="s">
-        <v>52</v>
-      </c>
       <c r="G29" s="1">
-        <v>42603</v>
-      </c>
-      <c r="H29" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H29" s="1">
+        <v>8</v>
+      </c>
+      <c r="I29" s="1">
+        <v>17</v>
+      </c>
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1356,25 +1536,31 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
         <v>23</v>
       </c>
       <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
         <v>51</v>
       </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
       <c r="G30" s="1">
-        <v>42603</v>
-      </c>
-      <c r="H30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="H30" s="1">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1">
+        <v>17</v>
+      </c>
+      <c r="J30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1382,26 +1568,32 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
       </c>
       <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
         <v>51</v>
       </c>
-      <c r="F31" t="s">
-        <v>52</v>
-      </c>
       <c r="G31" s="1">
-        <v>42603</v>
-      </c>
-      <c r="H31" t="s">
-        <v>32</v>
+        <v>2016</v>
+      </c>
+      <c r="H31" s="1">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1">
+        <v>17</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J31"/>
+  <autoFilter ref="A1:L31"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1416,9 +1608,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,10 +1618,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>